<commit_message>
Done prototype SRS 2.0
</commit_message>
<xml_diff>
--- a/CM_Plan/Design/Database Desgin/Database_V1.4.xlsx
+++ b/CM_Plan/Design/Database Desgin/Database_V1.4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t xml:space="preserve">Member</t>
   </si>
@@ -106,19 +106,13 @@
     <t xml:space="preserve">Hours</t>
   </si>
   <si>
-    <t xml:space="preserve">TimeLog</t>
+    <t xml:space="preserve">DateLog</t>
   </si>
   <si>
     <t xml:space="preserve">StatusFeedBack</t>
   </si>
   <si>
     <t xml:space="preserve">AccountFeedBack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DateFeedBack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ContentFeedBack</t>
   </si>
 </sst>
 </file>
@@ -128,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -157,6 +151,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -208,7 +208,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,6 +234,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,13 +297,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>1440</xdr:colOff>
       <xdr:row>211</xdr:row>
-      <xdr:rowOff>117000</xdr:rowOff>
+      <xdr:rowOff>117360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>35280</xdr:colOff>
       <xdr:row>211</xdr:row>
-      <xdr:rowOff>117360</xdr:rowOff>
+      <xdr:rowOff>117720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -308,7 +312,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3031560" y="42321960"/>
+          <a:off x="3031560" y="42322320"/>
           <a:ext cx="1544400" cy="360"/>
         </a:xfrm>
         <a:custGeom>
@@ -332,7 +336,6 @@
           <a:solidFill>
             <a:srgbClr val="4a7ebb"/>
           </a:solidFill>
-          <a:round/>
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
@@ -354,9 +357,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>25200</xdr:colOff>
+      <xdr:colOff>25560</xdr:colOff>
       <xdr:row>211</xdr:row>
-      <xdr:rowOff>92160</xdr:rowOff>
+      <xdr:rowOff>92520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -371,8 +374,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5895720" y="42297120"/>
-          <a:ext cx="1627560" cy="191520"/>
+          <a:off x="5896440" y="42297480"/>
+          <a:ext cx="1627200" cy="191160"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -395,7 +398,6 @@
           <a:solidFill>
             <a:srgbClr val="4a7ebb"/>
           </a:solidFill>
-          <a:round/>
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
@@ -419,13 +421,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>1440</xdr:colOff>
       <xdr:row>211</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>100800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>28800</xdr:colOff>
+      <xdr:colOff>28440</xdr:colOff>
       <xdr:row>223</xdr:row>
-      <xdr:rowOff>83520</xdr:rowOff>
+      <xdr:rowOff>83160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -434,8 +436,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8971920" y="42305400"/>
-          <a:ext cx="1627560" cy="2383560"/>
+          <a:off x="8972640" y="42305760"/>
+          <a:ext cx="1627200" cy="2382840"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -458,7 +460,6 @@
           <a:solidFill>
             <a:srgbClr val="4a7ebb"/>
           </a:solidFill>
-          <a:round/>
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
@@ -480,13 +481,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>17280</xdr:colOff>
+      <xdr:colOff>16560</xdr:colOff>
       <xdr:row>215</xdr:row>
       <xdr:rowOff>73800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>11880</xdr:colOff>
+      <xdr:colOff>10800</xdr:colOff>
       <xdr:row>222</xdr:row>
       <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
@@ -498,7 +499,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1">
           <a:off x="8987760" y="43079040"/>
-          <a:ext cx="1594800" cy="1467720"/>
+          <a:ext cx="1594440" cy="1467720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -521,7 +522,6 @@
           <a:solidFill>
             <a:srgbClr val="4a7ebb"/>
           </a:solidFill>
-          <a:round/>
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
@@ -543,15 +543,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>220</xdr:row>
-      <xdr:rowOff>83880</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>37080</xdr:colOff>
       <xdr:row>223</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -560,8 +560,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5871960" y="44089200"/>
-          <a:ext cx="1635840" cy="624600"/>
+          <a:off x="5872680" y="44089560"/>
+          <a:ext cx="1635480" cy="623880"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -584,7 +584,6 @@
           <a:solidFill>
             <a:srgbClr val="4a7ebb"/>
           </a:solidFill>
-          <a:round/>
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
@@ -608,7 +607,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>9360</xdr:colOff>
       <xdr:row>211</xdr:row>
-      <xdr:rowOff>117000</xdr:rowOff>
+      <xdr:rowOff>117360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
@@ -623,8 +622,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3039480" y="42321960"/>
-          <a:ext cx="1527840" cy="2183400"/>
+          <a:off x="3039480" y="42322320"/>
+          <a:ext cx="1527840" cy="2183040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -647,7 +646,6 @@
           <a:solidFill>
             <a:srgbClr val="4a7ebb"/>
           </a:solidFill>
-          <a:round/>
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
@@ -677,7 +675,7 @@
   <dimension ref="C211:L236"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A207" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F217" activeCellId="0" sqref="F217"/>
+      <selection pane="topLeft" activeCell="F229" activeCellId="0" sqref="F229:F235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -900,44 +898,38 @@
         <v>27</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C229" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F229" s="4"/>
-    </row>
-    <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F229" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C230" s="4"/>
-      <c r="F230" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F231" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F232" s="4" t="s">
+    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F232" s="4"/>
+    </row>
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F233" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F233" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F234" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F235" s="4"/>
-    </row>
-    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F236" s="3"/>
-    </row>
+    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F234" s="4"/>
+    </row>
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F235" s="3"/>
+    </row>
+    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lên khung SRS cho Team viết
</commit_message>
<xml_diff>
--- a/CM_Plan/Design/Database Desgin/Database_V1.4.xlsx
+++ b/CM_Plan/Design/Database Desgin/Database_V1.4.xlsx
@@ -1,260 +1,825 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView windowWidth="22665" windowHeight="12915" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
-    <t xml:space="preserve">Member</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Join Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FullName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RoleProject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Join Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finish Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Log Work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create By</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID LogWork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type Work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DateLog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StatusFeedBack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AccountFeedBack</t>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>1-n</t>
+  </si>
+  <si>
+    <t>Join Project</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>ID Project</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>RoleProject</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Join Date</t>
+  </si>
+  <si>
+    <t>Finish Date</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ID Product</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Phases</t>
+  </si>
+  <si>
+    <t>Log Work</t>
+  </si>
+  <si>
+    <t>Create By</t>
+  </si>
+  <si>
+    <t>ID LogWork</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Type Work</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>DateLog</t>
+  </si>
+  <si>
+    <t>StatusFeedBack</t>
+  </si>
+  <si>
+    <t>AccountFeedBack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+  <borders count="10">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -265,22 +830,24 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>231480</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>186840</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>15390</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 80" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 80"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:stretch/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="4772160" cy="986760"/>
+          <a:ext cx="4123055" cy="872490"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -307,18 +874,19 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3031560" y="42322320"/>
-          <a:ext cx="1544400" cy="360"/>
+          <a:off x="2598420" y="36292790"/>
+          <a:ext cx="1328420" cy="635"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
           <a:gdLst/>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="l" t="t" r="r" b="b"/>
           <a:pathLst>
             <a:path w="21600" h="21600">
@@ -334,9 +902,9 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
+            <a:srgbClr val="4A7EBB"/>
           </a:solidFill>
-          <a:tailEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -369,18 +937,19 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5896440" y="42297480"/>
-          <a:ext cx="1627200" cy="191160"/>
+          <a:off x="5057140" y="36268025"/>
+          <a:ext cx="1398270" cy="162560"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
           <a:gdLst/>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="l" t="t" r="r" b="b"/>
           <a:pathLst>
             <a:path w="21600" h="21600">
@@ -396,9 +965,9 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
+            <a:srgbClr val="4A7EBB"/>
           </a:solidFill>
-          <a:tailEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -431,18 +1000,19 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1"/>
+        <xdr:cNvPr id="5" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8972640" y="42305760"/>
-          <a:ext cx="1627200" cy="2382840"/>
+          <a:off x="7689850" y="36276280"/>
+          <a:ext cx="1398270" cy="2039620"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
           <a:gdLst/>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="l" t="t" r="r" b="b"/>
           <a:pathLst>
             <a:path w="21600" h="21600">
@@ -458,9 +1028,9 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
+            <a:srgbClr val="4A7EBB"/>
           </a:solidFill>
-          <a:tailEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -493,18 +1063,19 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1"/>
+        <xdr:cNvPr id="6" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="8987760" y="43079040"/>
-          <a:ext cx="1594440" cy="1467720"/>
+          <a:off x="7705090" y="36935410"/>
+          <a:ext cx="1365885" cy="1267460"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
           <a:gdLst/>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="l" t="t" r="r" b="b"/>
           <a:pathLst>
             <a:path w="21600" h="21600">
@@ -520,9 +1091,9 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
+            <a:srgbClr val="4A7EBB"/>
           </a:solidFill>
-          <a:tailEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -555,18 +1126,19 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1"/>
+        <xdr:cNvPr id="7" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5872680" y="44089560"/>
-          <a:ext cx="1635480" cy="623880"/>
+          <a:off x="5033010" y="37802820"/>
+          <a:ext cx="1407160" cy="538480"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
           <a:gdLst/>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="l" t="t" r="r" b="b"/>
           <a:pathLst>
             <a:path w="21600" h="21600">
@@ -582,9 +1154,9 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
+            <a:srgbClr val="4A7EBB"/>
           </a:solidFill>
-          <a:tailEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -617,18 +1189,19 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1"/>
+        <xdr:cNvPr id="8" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3039480" y="42322320"/>
-          <a:ext cx="1527840" cy="2183040"/>
+          <a:off x="2606040" y="36292790"/>
+          <a:ext cx="1311910" cy="1868805"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
           <a:gdLst/>
           <a:ahLst/>
+          <a:cxnLst/>
           <a:rect l="l" t="t" r="r" b="b"/>
           <a:pathLst>
             <a:path w="21600" h="21600">
@@ -644,9 +1217,9 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
+            <a:srgbClr val="4A7EBB"/>
           </a:solidFill>
-          <a:tailEnd len="med" type="triangle" w="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -667,32 +1240,285 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="C211:L236"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A207" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F229" activeCellId="0" sqref="F229:F235"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="J231" sqref="J231"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="9"/>
+    <col min="1" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="16.0833333333333" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="7.99166666666667" customWidth="1"/>
+    <col min="6" max="6" width="14.9583333333333" customWidth="1"/>
+    <col min="7" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="16.8666666666667" customWidth="1"/>
+    <col min="10" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="17.8333333333333" customWidth="1"/>
+    <col min="13" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" spans="3:9">
       <c r="C211" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +1532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" spans="3:9">
       <c r="C212" s="3" t="s">
         <v>4</v>
       </c>
@@ -720,7 +1546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" spans="3:9">
       <c r="C213" s="4" t="s">
         <v>6</v>
       </c>
@@ -731,7 +1557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" spans="3:9">
       <c r="C214" s="4" t="s">
         <v>8</v>
       </c>
@@ -742,7 +1568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" spans="3:12">
       <c r="C215" s="4"/>
       <c r="F215" s="4" t="s">
         <v>11</v>
@@ -754,7 +1580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" spans="3:12">
       <c r="C216" s="4" t="s">
         <v>14</v>
       </c>
@@ -768,7 +1594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" spans="3:12">
       <c r="C217" s="4" t="s">
         <v>17</v>
       </c>
@@ -779,29 +1605,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" spans="3:12">
       <c r="C218" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D218" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I218" s="0" t="s">
+      <c r="I218" t="s">
         <v>20</v>
       </c>
       <c r="L218" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" spans="3:12">
       <c r="C219" s="4"/>
-      <c r="F219" s="5"/>
+      <c r="F219" s="6"/>
       <c r="L219" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D220" s="6"/>
+    <row r="220" spans="4:12">
+      <c r="D220" s="5"/>
       <c r="F220" s="1" t="s">
         <v>21</v>
       </c>
@@ -812,7 +1638,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" spans="6:12">
       <c r="F221" s="3" t="s">
         <v>23</v>
       </c>
@@ -820,7 +1646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" spans="3:12">
       <c r="C222" s="1" t="s">
         <v>24</v>
       </c>
@@ -833,7 +1659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" spans="3:12">
       <c r="C223" s="3" t="s">
         <v>4</v>
       </c>
@@ -848,7 +1674,7 @@
       </c>
       <c r="L223" s="4"/>
     </row>
-    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" spans="3:12">
       <c r="C224" s="4" t="s">
         <v>6</v>
       </c>
@@ -862,7 +1688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" spans="3:12">
       <c r="C225" s="4" t="s">
         <v>8</v>
       </c>
@@ -874,14 +1700,14 @@
       </c>
       <c r="L225" s="4"/>
     </row>
-    <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" spans="3:9">
       <c r="C226" s="4"/>
       <c r="F226" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I226" s="4"/>
     </row>
-    <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" spans="3:9">
       <c r="C227" s="4" t="s">
         <v>14</v>
       </c>
@@ -890,7 +1716,7 @@
       </c>
       <c r="I227" s="4"/>
     </row>
-    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" spans="3:6">
       <c r="C228" s="4" t="s">
         <v>17</v>
       </c>
@@ -898,7 +1724,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" spans="3:6">
       <c r="C229" s="4" t="s">
         <v>19</v>
       </c>
@@ -906,38 +1732,36 @@
         <v>28</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" spans="3:6">
       <c r="C230" s="4"/>
-    </row>
-    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F230" s="8"/>
+    </row>
+    <row r="231" spans="6:6">
       <c r="F231" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" spans="6:6">
       <c r="F232" s="4"/>
     </row>
-    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" spans="6:6">
       <c r="F233" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" spans="6:6">
       <c r="F234" s="4"/>
     </row>
-    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" spans="6:6">
       <c r="F235" s="3"/>
     </row>
-    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="236" spans="6:6">
+      <c r="F236" s="8"/>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>